<commit_message>
organização das datas no grafico de cs
</commit_message>
<xml_diff>
--- a/Definitivo.xlsx
+++ b/Definitivo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\Programação\Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9F5338-C577-4061-8A82-C745CDD47C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E768352-6892-4740-AB37-B927F4933723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -634,13 +634,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -959,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U142" sqref="U142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +966,7 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" style="12" customWidth="1"/>
     <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1034,7 +1032,7 @@
       <c r="T1" t="s">
         <v>167</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="12" t="s">
         <v>168</v>
       </c>
       <c r="V1" t="s">
@@ -3442,7 +3440,7 @@
       <c r="T29">
         <v>0</v>
       </c>
-      <c r="U29" s="12">
+      <c r="U29" s="13">
         <v>1309.33</v>
       </c>
       <c r="V29">
@@ -3528,7 +3526,7 @@
       <c r="T30">
         <v>0</v>
       </c>
-      <c r="U30" s="12">
+      <c r="U30" s="13">
         <v>1309.33</v>
       </c>
       <c r="V30">
@@ -3614,7 +3612,7 @@
       <c r="T31">
         <v>0</v>
       </c>
-      <c r="U31" s="12">
+      <c r="U31" s="13">
         <v>1309.33</v>
       </c>
       <c r="V31">
@@ -3700,7 +3698,7 @@
       <c r="T32">
         <v>0</v>
       </c>
-      <c r="U32" s="12">
+      <c r="U32" s="13">
         <v>1309.33</v>
       </c>
       <c r="V32">
@@ -3786,7 +3784,7 @@
       <c r="T33">
         <v>0</v>
       </c>
-      <c r="U33" s="12">
+      <c r="U33" s="13">
         <v>6772.76</v>
       </c>
       <c r="V33">
@@ -3872,7 +3870,7 @@
       <c r="T34">
         <v>0</v>
       </c>
-      <c r="U34" s="12">
+      <c r="U34" s="13">
         <v>13260.77</v>
       </c>
       <c r="V34">
@@ -3958,7 +3956,7 @@
       <c r="T35">
         <v>0</v>
       </c>
-      <c r="U35" s="12">
+      <c r="U35" s="13">
         <v>23973.98</v>
       </c>
       <c r="V35">
@@ -4044,7 +4042,7 @@
       <c r="T36">
         <v>0</v>
       </c>
-      <c r="U36" s="12">
+      <c r="U36" s="13">
         <v>122425.32</v>
       </c>
       <c r="V36">
@@ -4130,7 +4128,7 @@
       <c r="T37">
         <v>0</v>
       </c>
-      <c r="U37" s="12">
+      <c r="U37" s="13">
         <v>222538.77</v>
       </c>
       <c r="V37">
@@ -4216,7 +4214,7 @@
       <c r="T38">
         <v>0</v>
       </c>
-      <c r="U38" s="12">
+      <c r="U38" s="13">
         <v>21889.65</v>
       </c>
       <c r="V38">
@@ -4302,7 +4300,7 @@
       <c r="T39">
         <v>0</v>
       </c>
-      <c r="U39" s="12">
+      <c r="U39" s="13">
         <v>71698.91</v>
       </c>
       <c r="V39">
@@ -4388,7 +4386,7 @@
       <c r="T40">
         <v>0</v>
       </c>
-      <c r="U40" s="12">
+      <c r="U40" s="13">
         <v>164820.20000000001</v>
       </c>
       <c r="V40">
@@ -4474,7 +4472,7 @@
       <c r="T41">
         <v>0</v>
       </c>
-      <c r="U41" s="12">
+      <c r="U41" s="13">
         <v>297748.49</v>
       </c>
       <c r="V41">
@@ -4560,7 +4558,7 @@
       <c r="T42">
         <v>0</v>
       </c>
-      <c r="U42" s="12">
+      <c r="U42" s="13">
         <v>332547.96000000002</v>
       </c>
       <c r="V42">
@@ -4646,7 +4644,7 @@
       <c r="T43">
         <v>0</v>
       </c>
-      <c r="U43" s="12">
+      <c r="U43" s="13">
         <v>482987.23</v>
       </c>
       <c r="V43">
@@ -4732,7 +4730,7 @@
       <c r="T44">
         <v>0</v>
       </c>
-      <c r="U44" s="12">
+      <c r="U44" s="13">
         <v>520402.96</v>
       </c>
       <c r="V44">
@@ -4818,7 +4816,7 @@
       <c r="T45">
         <v>0</v>
       </c>
-      <c r="U45" s="12">
+      <c r="U45" s="13">
         <v>591825.81999999995</v>
       </c>
       <c r="V45">
@@ -4904,7 +4902,7 @@
       <c r="T46">
         <v>0</v>
       </c>
-      <c r="U46" s="12">
+      <c r="U46" s="13">
         <v>648901.71</v>
       </c>
       <c r="V46">
@@ -4990,7 +4988,7 @@
       <c r="T47">
         <v>0</v>
       </c>
-      <c r="U47" s="12">
+      <c r="U47" s="13">
         <v>731668.88</v>
       </c>
       <c r="V47">
@@ -5076,7 +5074,7 @@
       <c r="T48">
         <v>0</v>
       </c>
-      <c r="U48" s="12">
+      <c r="U48" s="13">
         <v>1331452.76</v>
       </c>
       <c r="V48">
@@ -5162,7 +5160,7 @@
       <c r="T49">
         <v>0</v>
       </c>
-      <c r="U49" s="12">
+      <c r="U49" s="13">
         <v>1461869.54</v>
       </c>
       <c r="V49">
@@ -5248,7 +5246,7 @@
       <c r="T50">
         <v>0</v>
       </c>
-      <c r="U50" s="12">
+      <c r="U50" s="13">
         <v>81389.25</v>
       </c>
       <c r="V50">
@@ -5334,7 +5332,7 @@
       <c r="T51">
         <v>0</v>
       </c>
-      <c r="U51" s="12">
+      <c r="U51" s="13">
         <v>122770.38</v>
       </c>
       <c r="V51">
@@ -5420,7 +5418,7 @@
       <c r="T52">
         <v>0</v>
       </c>
-      <c r="U52" s="12">
+      <c r="U52" s="13">
         <v>669657.65</v>
       </c>
       <c r="V52">
@@ -5506,7 +5504,7 @@
       <c r="T53">
         <v>0</v>
       </c>
-      <c r="U53" s="12">
+      <c r="U53" s="13">
         <v>754716.57</v>
       </c>
       <c r="V53">
@@ -5592,7 +5590,7 @@
       <c r="T54">
         <v>0</v>
       </c>
-      <c r="U54" s="12">
+      <c r="U54" s="13">
         <v>816811.22</v>
       </c>
       <c r="V54">
@@ -5678,7 +5676,7 @@
       <c r="T55">
         <v>0</v>
       </c>
-      <c r="U55" s="12">
+      <c r="U55" s="13">
         <v>971753.74</v>
       </c>
       <c r="V55">
@@ -5764,7 +5762,7 @@
       <c r="T56">
         <v>0</v>
       </c>
-      <c r="U56" s="12">
+      <c r="U56" s="13">
         <v>1038665.2</v>
       </c>
       <c r="V56">
@@ -5850,7 +5848,7 @@
       <c r="T57">
         <v>0</v>
       </c>
-      <c r="U57" s="12">
+      <c r="U57" s="13">
         <v>1645629.14</v>
       </c>
       <c r="V57">
@@ -5936,7 +5934,7 @@
       <c r="T58">
         <v>0</v>
       </c>
-      <c r="U58" s="12">
+      <c r="U58" s="13">
         <v>1707689.43</v>
       </c>
       <c r="V58">
@@ -6022,7 +6020,7 @@
       <c r="T59">
         <v>0</v>
       </c>
-      <c r="U59" s="12">
+      <c r="U59" s="13">
         <v>1923818.96</v>
       </c>
       <c r="V59">
@@ -6108,7 +6106,7 @@
       <c r="T60">
         <v>0</v>
       </c>
-      <c r="U60" s="12">
+      <c r="U60" s="13">
         <v>2571492.64</v>
       </c>
       <c r="V60">
@@ -6194,7 +6192,7 @@
       <c r="T61">
         <v>0</v>
       </c>
-      <c r="U61" s="12">
+      <c r="U61" s="13">
         <v>2712515.01</v>
       </c>
       <c r="V61">
@@ -6280,7 +6278,7 @@
       <c r="T62">
         <v>0</v>
       </c>
-      <c r="U62" s="12">
+      <c r="U62" s="13">
         <v>109366.62</v>
       </c>
       <c r="V62">
@@ -6366,7 +6364,7 @@
       <c r="T63">
         <v>0</v>
       </c>
-      <c r="U63" s="12">
+      <c r="U63" s="13">
         <v>219315.47</v>
       </c>
       <c r="V63">
@@ -6452,7 +6450,7 @@
       <c r="T64">
         <v>0</v>
       </c>
-      <c r="U64" s="12">
+      <c r="U64" s="13">
         <v>882518.74</v>
       </c>
       <c r="V64">
@@ -6538,7 +6536,7 @@
       <c r="T65">
         <v>0</v>
       </c>
-      <c r="U65" s="12">
+      <c r="U65" s="13">
         <v>1355408.95</v>
       </c>
       <c r="V65">
@@ -6624,7 +6622,7 @@
       <c r="T66">
         <v>0</v>
       </c>
-      <c r="U66" s="12">
+      <c r="U66" s="13">
         <v>1609173.1</v>
       </c>
       <c r="V66">
@@ -6710,7 +6708,7 @@
       <c r="T67">
         <v>0</v>
       </c>
-      <c r="U67" s="12">
+      <c r="U67" s="13">
         <v>2226852.1800000002</v>
       </c>
       <c r="V67">
@@ -6796,7 +6794,7 @@
       <c r="T68">
         <v>0</v>
       </c>
-      <c r="U68" s="12">
+      <c r="U68" s="13">
         <v>3107961.9</v>
       </c>
       <c r="V68">
@@ -6882,7 +6880,7 @@
       <c r="T69">
         <v>0</v>
       </c>
-      <c r="U69" s="12">
+      <c r="U69" s="13">
         <v>3855994.04</v>
       </c>
       <c r="V69">
@@ -6968,7 +6966,7 @@
       <c r="T70">
         <v>0</v>
       </c>
-      <c r="U70" s="12">
+      <c r="U70" s="13">
         <v>4431774.63</v>
       </c>
       <c r="V70">
@@ -7054,7 +7052,7 @@
       <c r="T71">
         <v>0</v>
       </c>
-      <c r="U71" s="12">
+      <c r="U71" s="13">
         <v>4846558.66</v>
       </c>
       <c r="V71">
@@ -7140,7 +7138,7 @@
       <c r="T72">
         <v>0</v>
       </c>
-      <c r="U72" s="12">
+      <c r="U72" s="13">
         <v>6040571.0499999998</v>
       </c>
       <c r="V72">
@@ -7226,7 +7224,7 @@
       <c r="T73">
         <v>0</v>
       </c>
-      <c r="U73" s="12">
+      <c r="U73" s="13">
         <v>7343809.6799999997</v>
       </c>
       <c r="V73">
@@ -7312,7 +7310,7 @@
       <c r="T74">
         <v>0</v>
       </c>
-      <c r="U74" s="12">
+      <c r="U74" s="13">
         <v>703550.83</v>
       </c>
       <c r="V74">
@@ -7398,7 +7396,7 @@
       <c r="T75">
         <v>0</v>
       </c>
-      <c r="U75" s="12">
+      <c r="U75" s="13">
         <v>1312413.95</v>
       </c>
       <c r="V75">
@@ -7484,7 +7482,7 @@
       <c r="T76">
         <v>0</v>
       </c>
-      <c r="U76" s="12">
+      <c r="U76" s="13">
         <v>1789987.13</v>
       </c>
       <c r="V76">
@@ -7570,7 +7568,7 @@
       <c r="T77">
         <v>0</v>
       </c>
-      <c r="U77" s="12">
+      <c r="U77" s="13">
         <v>4378457.7699999996</v>
       </c>
       <c r="V77">
@@ -7656,7 +7654,7 @@
       <c r="T78">
         <v>0</v>
       </c>
-      <c r="U78" s="12">
+      <c r="U78" s="13">
         <v>5960841.9400000004</v>
       </c>
       <c r="V78">
@@ -7742,7 +7740,7 @@
       <c r="T79">
         <v>0</v>
       </c>
-      <c r="U79" s="12">
+      <c r="U79" s="13">
         <v>7203783.9299999997</v>
       </c>
       <c r="V79">
@@ -7828,7 +7826,7 @@
       <c r="T80">
         <v>0</v>
       </c>
-      <c r="U80" s="12">
+      <c r="U80" s="13">
         <v>11128892.18</v>
       </c>
       <c r="V80">
@@ -7914,7 +7912,7 @@
       <c r="T81">
         <v>0</v>
       </c>
-      <c r="U81" s="12">
+      <c r="U81" s="13">
         <v>11572328.16</v>
       </c>
       <c r="V81">
@@ -8000,7 +7998,7 @@
       <c r="T82">
         <v>0</v>
       </c>
-      <c r="U82" s="12">
+      <c r="U82" s="13">
         <v>12551395.25</v>
       </c>
       <c r="V82">
@@ -8086,7 +8084,7 @@
       <c r="T83">
         <v>0</v>
       </c>
-      <c r="U83" s="12">
+      <c r="U83" s="13">
         <v>14874091.83</v>
       </c>
       <c r="V83">
@@ -8172,7 +8170,7 @@
       <c r="T84">
         <v>0</v>
       </c>
-      <c r="U84" s="12">
+      <c r="U84" s="13">
         <v>16594388.42</v>
       </c>
       <c r="V84">
@@ -8258,7 +8256,7 @@
       <c r="T85">
         <v>22.3</v>
       </c>
-      <c r="U85" s="12">
+      <c r="U85" s="13">
         <v>19828410.899999999</v>
       </c>
       <c r="V85">
@@ -8344,7 +8342,7 @@
       <c r="T86">
         <v>0.2</v>
       </c>
-      <c r="U86" s="12">
+      <c r="U86" s="13">
         <v>3674065.16</v>
       </c>
       <c r="V86">
@@ -8430,7 +8428,7 @@
       <c r="T87">
         <v>-8.6</v>
       </c>
-      <c r="U87" s="12">
+      <c r="U87" s="13">
         <v>4222397.51</v>
       </c>
       <c r="V87">
@@ -8516,7 +8514,7 @@
       <c r="T88">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="U88" s="12">
+      <c r="U88" s="13">
         <v>4653798.38</v>
       </c>
       <c r="V88">
@@ -8602,7 +8600,7 @@
       <c r="T89">
         <v>5</v>
       </c>
-      <c r="U89" s="12">
+      <c r="U89" s="13">
         <v>5431545.3600000003</v>
       </c>
       <c r="V89">
@@ -8688,7 +8686,7 @@
       <c r="T90">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="U90" s="12">
+      <c r="U90" s="13">
         <v>6255335.6500000004</v>
       </c>
       <c r="V90">
@@ -8774,7 +8772,7 @@
       <c r="T91">
         <v>0</v>
       </c>
-      <c r="U91" s="12">
+      <c r="U91" s="13">
         <v>9066567.9100000001</v>
       </c>
       <c r="V91">
@@ -8860,7 +8858,7 @@
       <c r="T92">
         <v>-15.1</v>
       </c>
-      <c r="U92" s="12">
+      <c r="U92" s="13">
         <v>11881322.24</v>
       </c>
       <c r="V92">
@@ -8946,7 +8944,7 @@
       <c r="T93">
         <v>3.5</v>
       </c>
-      <c r="U93" s="12">
+      <c r="U93" s="13">
         <v>12177797.380000001</v>
       </c>
       <c r="V93">
@@ -9032,7 +9030,7 @@
       <c r="T94">
         <v>27.2</v>
       </c>
-      <c r="U94" s="12">
+      <c r="U94" s="13">
         <v>13517829.67</v>
       </c>
       <c r="V94">
@@ -9118,7 +9116,7 @@
       <c r="T95">
         <v>-12.4</v>
       </c>
-      <c r="U95" s="12">
+      <c r="U95" s="13">
         <v>15955291.33</v>
       </c>
       <c r="V95">
@@ -9204,7 +9202,7 @@
       <c r="T96">
         <v>-16</v>
       </c>
-      <c r="U96" s="12">
+      <c r="U96" s="13">
         <v>17789627.760000002</v>
       </c>
       <c r="V96">
@@ -9290,7 +9288,7 @@
       <c r="T97">
         <v>28</v>
       </c>
-      <c r="U97" s="12">
+      <c r="U97" s="13">
         <v>21706143.07</v>
       </c>
       <c r="V97">
@@ -9376,7 +9374,7 @@
       <c r="T98">
         <v>-9</v>
       </c>
-      <c r="U98" s="12">
+      <c r="U98" s="13">
         <v>2269332.4</v>
       </c>
       <c r="V98">
@@ -9462,7 +9460,7 @@
       <c r="T99">
         <v>9.6999999999999993</v>
       </c>
-      <c r="U99" s="12">
+      <c r="U99" s="13">
         <v>3051946.94</v>
       </c>
       <c r="V99">
@@ -9548,7 +9546,7 @@
       <c r="T100">
         <v>-16.5</v>
       </c>
-      <c r="U100" s="12">
+      <c r="U100" s="13">
         <v>6343374.9900000002</v>
       </c>
       <c r="V100">
@@ -9634,7 +9632,7 @@
       <c r="T101">
         <v>10.6</v>
       </c>
-      <c r="U101" s="12">
+      <c r="U101" s="13">
         <v>7175581.3899999997</v>
       </c>
       <c r="V101">
@@ -9720,7 +9718,7 @@
       <c r="T102">
         <v>-11.7</v>
       </c>
-      <c r="U102" s="12">
+      <c r="U102" s="13">
         <v>9033439.8599999994</v>
       </c>
       <c r="V102">
@@ -9806,7 +9804,7 @@
       <c r="T103">
         <v>3.5</v>
       </c>
-      <c r="U103" s="12">
+      <c r="U103" s="13">
         <v>11085702.880000001</v>
       </c>
       <c r="V103">
@@ -9892,7 +9890,7 @@
       <c r="T104">
         <v>8.4</v>
       </c>
-      <c r="U104" s="12">
+      <c r="U104" s="13">
         <v>13103512.65</v>
       </c>
       <c r="V104">
@@ -9978,7 +9976,7 @@
       <c r="T105">
         <v>-5.8</v>
       </c>
-      <c r="U105" s="12">
+      <c r="U105" s="13">
         <v>14056493.49</v>
       </c>
       <c r="V105">
@@ -10064,7 +10062,7 @@
       <c r="T106">
         <v>42.4</v>
       </c>
-      <c r="U106" s="12">
+      <c r="U106" s="13">
         <v>17472086.800000001</v>
       </c>
       <c r="V106">
@@ -10150,7 +10148,7 @@
       <c r="T107">
         <v>-22.4</v>
       </c>
-      <c r="U107" s="12">
+      <c r="U107" s="13">
         <v>18934213.420000002</v>
       </c>
       <c r="V107">
@@ -10236,7 +10234,7 @@
       <c r="T108">
         <v>-14.7</v>
       </c>
-      <c r="U108" s="12">
+      <c r="U108" s="13">
         <v>20983098.93</v>
       </c>
       <c r="V108">
@@ -10322,7 +10320,7 @@
       <c r="T109">
         <v>37.5</v>
       </c>
-      <c r="U109" s="12">
+      <c r="U109" s="13">
         <v>25578825.949999999</v>
       </c>
       <c r="V109">
@@ -10408,7 +10406,7 @@
       <c r="T110">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="U110" s="12">
+      <c r="U110" s="13">
         <v>853086.74</v>
       </c>
       <c r="V110">
@@ -10494,7 +10492,7 @@
       <c r="T111">
         <v>14.1</v>
       </c>
-      <c r="U111" s="12">
+      <c r="U111" s="13">
         <v>1085693.5</v>
       </c>
       <c r="V111">
@@ -10580,7 +10578,7 @@
       <c r="T112">
         <v>-14.7</v>
       </c>
-      <c r="U112" s="12">
+      <c r="U112" s="13">
         <v>4484567.3499999996</v>
       </c>
       <c r="V112">
@@ -10666,7 +10664,7 @@
       <c r="T113">
         <v>11.2</v>
       </c>
-      <c r="U113" s="12">
+      <c r="U113" s="13">
         <v>6143408.9000000004</v>
       </c>
       <c r="V113">
@@ -10752,7 +10750,7 @@
       <c r="T114">
         <v>-13.3</v>
       </c>
-      <c r="U114" s="12">
+      <c r="U114" s="13">
         <v>7108982.2599999998</v>
       </c>
       <c r="V114">
@@ -10838,7 +10836,7 @@
       <c r="T115">
         <v>-23.5</v>
       </c>
-      <c r="U115" s="12">
+      <c r="U115" s="13">
         <v>9665600.8200000003</v>
       </c>
       <c r="V115">
@@ -10924,7 +10922,7 @@
       <c r="T116">
         <v>26.2</v>
       </c>
-      <c r="U116" s="12">
+      <c r="U116" s="13">
         <v>12538772.5</v>
       </c>
       <c r="V116">
@@ -11010,7 +11008,7 @@
       <c r="T117">
         <v>-9.9</v>
       </c>
-      <c r="U117" s="12">
+      <c r="U117" s="13">
         <v>12769762.66</v>
       </c>
       <c r="V117">
@@ -11096,7 +11094,7 @@
       <c r="T118">
         <v>56.2</v>
       </c>
-      <c r="U118" s="12">
+      <c r="U118" s="13">
         <v>15917600.130000001</v>
       </c>
       <c r="V118">
@@ -11182,7 +11180,7 @@
       <c r="T119">
         <v>-24.2</v>
       </c>
-      <c r="U119" s="12">
+      <c r="U119" s="13">
         <v>17238507.620000001</v>
       </c>
       <c r="V119">
@@ -11268,7 +11266,7 @@
       <c r="T120">
         <v>-14.4</v>
       </c>
-      <c r="U120" s="12">
+      <c r="U120" s="13">
         <v>18919910.899999999</v>
       </c>
       <c r="V120">
@@ -11354,7 +11352,7 @@
       <c r="T121">
         <v>27</v>
       </c>
-      <c r="U121" s="12">
+      <c r="U121" s="13">
         <v>24410889.960000001</v>
       </c>
       <c r="V121">
@@ -11440,7 +11438,7 @@
       <c r="T122">
         <v>21.7</v>
       </c>
-      <c r="U122" s="12">
+      <c r="U122" s="13">
         <v>351510.31</v>
       </c>
       <c r="V122">
@@ -11526,7 +11524,7 @@
       <c r="T123">
         <v>1.7</v>
       </c>
-      <c r="U123" s="12">
+      <c r="U123" s="13">
         <v>856920.23</v>
       </c>
       <c r="V123">
@@ -11612,7 +11610,7 @@
       <c r="T124">
         <v>9.6</v>
       </c>
-      <c r="U124" s="12">
+      <c r="U124" s="13">
         <v>1418856.88</v>
       </c>
       <c r="V124">
@@ -11698,7 +11696,7 @@
       <c r="T125">
         <v>-5.9</v>
       </c>
-      <c r="U125" s="12">
+      <c r="U125" s="13">
         <v>3411472.29</v>
       </c>
       <c r="V125">
@@ -11784,7 +11782,7 @@
       <c r="T126">
         <v>12.4</v>
       </c>
-      <c r="U126" s="12">
+      <c r="U126" s="13">
         <v>4401347.3099999996</v>
       </c>
       <c r="V126">
@@ -11870,7 +11868,7 @@
       <c r="T127">
         <v>-5.4</v>
       </c>
-      <c r="U127" s="12">
+      <c r="U127" s="13">
         <v>5292478.57</v>
       </c>
       <c r="V127">
@@ -11956,7 +11954,7 @@
       <c r="T128">
         <v>5.4</v>
       </c>
-      <c r="U128" s="12">
+      <c r="U128" s="13">
         <v>5923904.8300000001</v>
       </c>
       <c r="V128">
@@ -12042,7 +12040,7 @@
       <c r="T129">
         <v>-5.3</v>
       </c>
-      <c r="U129" s="12">
+      <c r="U129" s="13">
         <v>7030944.4699999997</v>
       </c>
       <c r="V129">
@@ -12128,7 +12126,7 @@
       <c r="T130">
         <v>27.3</v>
       </c>
-      <c r="U130" s="12">
+      <c r="U130" s="13">
         <v>7938994.1799999997</v>
       </c>
       <c r="V130">
@@ -12214,7 +12212,7 @@
       <c r="T131">
         <v>-29.5</v>
       </c>
-      <c r="U131" s="12">
+      <c r="U131" s="13">
         <v>9901760.1400000006</v>
       </c>
       <c r="V131">
@@ -12300,7 +12298,7 @@
       <c r="T132">
         <v>-20.5</v>
       </c>
-      <c r="U132" s="12">
+      <c r="U132" s="13">
         <v>10856319.77</v>
       </c>
       <c r="V132">
@@ -12386,7 +12384,7 @@
       <c r="T133">
         <v>77.099999999999994</v>
       </c>
-      <c r="U133" s="12">
+      <c r="U133" s="13">
         <v>16625485.720000001</v>
       </c>
       <c r="V133">
@@ -12472,7 +12470,7 @@
       <c r="T134">
         <v>-12</v>
       </c>
-      <c r="U134" s="12">
+      <c r="U134" s="13">
         <v>1495367.34</v>
       </c>
       <c r="V134">
@@ -12558,7 +12556,7 @@
       <c r="T135">
         <v>-0.2</v>
       </c>
-      <c r="U135" s="12">
+      <c r="U135" s="13">
         <v>2742266.93</v>
       </c>
       <c r="V135">
@@ -12644,7 +12642,7 @@
       <c r="T136">
         <v>4.8</v>
       </c>
-      <c r="U136" s="12">
+      <c r="U136" s="13">
         <v>3074116.59</v>
       </c>
       <c r="V136">
@@ -12730,7 +12728,7 @@
       <c r="T137">
         <v>10.8</v>
       </c>
-      <c r="U137" s="12">
+      <c r="U137" s="13">
         <v>4592940.5</v>
       </c>
       <c r="V137">
@@ -12816,7 +12814,7 @@
       <c r="T138">
         <v>-15.2</v>
       </c>
-      <c r="U138" s="12">
+      <c r="U138" s="13">
         <v>5699314.1799999997</v>
       </c>
       <c r="V138">
@@ -12988,7 +12986,7 @@
       <c r="T140">
         <v>2.8</v>
       </c>
-      <c r="U140" s="12">
+      <c r="U140" s="13">
         <v>8318802.79</v>
       </c>
       <c r="V140">
@@ -13074,7 +13072,7 @@
       <c r="T141">
         <v>-22.2</v>
       </c>
-      <c r="U141" s="12">
+      <c r="U141" s="13">
         <v>8492996.6999999993</v>
       </c>
       <c r="V141">
@@ -13160,7 +13158,7 @@
       <c r="T142">
         <v>94</v>
       </c>
-      <c r="U142" s="12">
+      <c r="U142" s="13">
         <v>12203979.98</v>
       </c>
       <c r="V142">
@@ -13246,7 +13244,7 @@
       <c r="T143">
         <v>-50.8</v>
       </c>
-      <c r="U143" s="12">
+      <c r="U143" s="13">
         <v>13093092.5</v>
       </c>
       <c r="V143">
@@ -13332,7 +13330,7 @@
       <c r="T144">
         <v>-7.2</v>
       </c>
-      <c r="U144" s="12">
+      <c r="U144" s="13">
         <v>16619240.5</v>
       </c>
       <c r="V144">
@@ -13418,7 +13416,7 @@
       <c r="T145">
         <v>93.9</v>
       </c>
-      <c r="U145" s="12">
+      <c r="U145" s="13">
         <v>21319818.539999999</v>
       </c>
       <c r="V145">
@@ -13504,7 +13502,7 @@
       <c r="T146">
         <v>-27.3</v>
       </c>
-      <c r="U146" s="12">
+      <c r="U146" s="13">
         <v>390051.6</v>
       </c>
       <c r="V146">
@@ -13590,7 +13588,7 @@
       <c r="T147">
         <v>2.6</v>
       </c>
-      <c r="U147" s="12">
+      <c r="U147" s="13">
         <v>1936275.95</v>
       </c>
       <c r="V147">
@@ -13676,7 +13674,7 @@
       <c r="T148">
         <v>-72.8</v>
       </c>
-      <c r="U148" s="12">
+      <c r="U148" s="13">
         <v>2781319.21</v>
       </c>
       <c r="V148">
@@ -13759,7 +13757,7 @@
       <c r="T149">
         <v>0</v>
       </c>
-      <c r="U149" s="12">
+      <c r="U149" s="13">
         <v>3879519.85</v>
       </c>
       <c r="V149">

</xml_diff>